<commit_message>
fix dept code lookup
</commit_message>
<xml_diff>
--- a/billy_penn/data/dept_names_lookup.xlsx
+++ b/billy_penn/data/dept_names_lookup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/Software/billy-penn/billy_penn/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9ADA37-8F35-6F4D-81D0-A40E590F6A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C09160-6D52-1F43-A2A4-478785D0A2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1429,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B208" sqref="B208"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1462,7 +1462,7 @@
         <v>176</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f t="shared" ref="D2:D44" si="0">_xlfn.CONCAT(B2,C2)</f>
+        <f t="shared" ref="D2:D65" si="0">IF(C2 &lt;&gt; "",_xlfn.CONCAT(B2,_xlfn.CONCAT("-",C2)),B2)</f>
         <v>01</v>
       </c>
     </row>
@@ -1622,7 +1622,7 @@
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>04911</v>
+        <v>04-911</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1649,7 +1649,7 @@
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>05S</v>
+        <v>05-S</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1664,7 +1664,7 @@
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>05S</v>
+        <v>05-S</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>05S</v>
+        <v>05-S</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="D38" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>10LS</v>
+        <v>10-LS</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>10LS</v>
+        <v>10-LS</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1940,7 +1940,7 @@
       </c>
       <c r="D40" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>10LS</v>
+        <v>10-LS</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1955,7 +1955,7 @@
       </c>
       <c r="D41" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>10LS</v>
+        <v>10-LS</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1994,7 +1994,7 @@
       </c>
       <c r="D44" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>12D</v>
+        <v>12-D</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2008,8 +2008,8 @@
         <v>218</v>
       </c>
       <c r="D45" s="3" t="str">
-        <f t="shared" ref="D45:D82" si="1">_xlfn.CONCAT(B45,C45)</f>
-        <v>12S</v>
+        <f t="shared" si="0"/>
+        <v>12-S</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2023,8 +2023,8 @@
         <v>218</v>
       </c>
       <c r="D46" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>12S</v>
+        <f t="shared" si="0"/>
+        <v>12-S</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2038,8 +2038,8 @@
         <v>218</v>
       </c>
       <c r="D47" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>12S</v>
+        <f t="shared" si="0"/>
+        <v>12-S</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2053,8 +2053,8 @@
         <v>240</v>
       </c>
       <c r="D48" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>12T</v>
+        <f t="shared" si="0"/>
+        <v>12-T</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2068,8 +2068,8 @@
         <v>240</v>
       </c>
       <c r="D49" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>12T</v>
+        <f t="shared" si="0"/>
+        <v>12-T</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2080,7 +2080,7 @@
         <v>199</v>
       </c>
       <c r="D50" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
@@ -2092,7 +2092,7 @@
         <v>239</v>
       </c>
       <c r="D51" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
@@ -2104,7 +2104,7 @@
         <v>221</v>
       </c>
       <c r="D52" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -2116,7 +2116,7 @@
         <v>221</v>
       </c>
       <c r="D53" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -2128,7 +2128,7 @@
         <v>221</v>
       </c>
       <c r="D54" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -2140,7 +2140,7 @@
         <v>221</v>
       </c>
       <c r="D55" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -2152,7 +2152,7 @@
         <v>221</v>
       </c>
       <c r="D56" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -2164,7 +2164,7 @@
         <v>221</v>
       </c>
       <c r="D57" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -2176,7 +2176,7 @@
         <v>222</v>
       </c>
       <c r="D58" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -2188,7 +2188,7 @@
         <v>221</v>
       </c>
       <c r="D59" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -2200,7 +2200,7 @@
         <v>221</v>
       </c>
       <c r="D60" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -2212,7 +2212,7 @@
         <v>230</v>
       </c>
       <c r="D61" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
@@ -2224,7 +2224,7 @@
         <v>230</v>
       </c>
       <c r="D62" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
@@ -2236,7 +2236,7 @@
         <v>231</v>
       </c>
       <c r="D63" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
@@ -2248,7 +2248,7 @@
         <v>230</v>
       </c>
       <c r="D64" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
@@ -2260,7 +2260,7 @@
         <v>189</v>
       </c>
       <c r="D65" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
@@ -2272,7 +2272,7 @@
         <v>189</v>
       </c>
       <c r="D66" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D66:D114" si="1">IF(C66 &lt;&gt; "",_xlfn.CONCAT(B66,_xlfn.CONCAT("-",C66)),B66)</f>
         <v>17</v>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="D69" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20SR</v>
+        <v>20-SR</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2327,7 +2327,7 @@
       </c>
       <c r="D70" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20SR</v>
+        <v>20-SR</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="D71" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20SS</v>
+        <v>20-SS</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2357,7 +2357,7 @@
       </c>
       <c r="D72" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20SS</v>
+        <v>20-SS</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2372,7 +2372,7 @@
       </c>
       <c r="D73" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20T</v>
+        <v>20-T</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2387,7 +2387,7 @@
       </c>
       <c r="D74" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20T</v>
+        <v>20-T</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2402,7 +2402,7 @@
       </c>
       <c r="D75" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20T</v>
+        <v>20-T</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2417,7 +2417,7 @@
       </c>
       <c r="D76" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20U</v>
+        <v>20-U</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2500,7 +2500,7 @@
         <v>223</v>
       </c>
       <c r="D83" s="3" t="str">
-        <f t="shared" ref="D83:D123" si="2">_xlfn.CONCAT(B83,C83)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
@@ -2512,7 +2512,7 @@
         <v>223</v>
       </c>
       <c r="D84" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
@@ -2524,7 +2524,7 @@
         <v>223</v>
       </c>
       <c r="D85" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
@@ -2536,7 +2536,7 @@
         <v>201</v>
       </c>
       <c r="D86" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
     </row>
@@ -2551,8 +2551,8 @@
         <v>202</v>
       </c>
       <c r="D87" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>25V</v>
+        <f t="shared" si="1"/>
+        <v>25-V</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2566,8 +2566,8 @@
         <v>202</v>
       </c>
       <c r="D88" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>25V</v>
+        <f t="shared" si="1"/>
+        <v>25-V</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2581,8 +2581,8 @@
         <v>202</v>
       </c>
       <c r="D89" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>25V</v>
+        <f t="shared" si="1"/>
+        <v>25-V</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2596,8 +2596,8 @@
         <v>202</v>
       </c>
       <c r="D90" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>25V</v>
+        <f t="shared" si="1"/>
+        <v>25-V</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2611,8 +2611,8 @@
         <v>202</v>
       </c>
       <c r="D91" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>25V</v>
+        <f t="shared" si="1"/>
+        <v>25-V</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2626,8 +2626,8 @@
         <v>202</v>
       </c>
       <c r="D92" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>25V</v>
+        <f t="shared" si="1"/>
+        <v>25-V</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2641,8 +2641,8 @@
         <v>202</v>
       </c>
       <c r="D93" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>25V</v>
+        <f t="shared" si="1"/>
+        <v>25-V</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2653,7 +2653,7 @@
         <v>211</v>
       </c>
       <c r="D94" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
     </row>
@@ -2665,7 +2665,7 @@
         <v>211</v>
       </c>
       <c r="D95" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
     </row>
@@ -2680,8 +2680,8 @@
         <v>212</v>
       </c>
       <c r="D96" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>26D</v>
+        <f t="shared" si="1"/>
+        <v>26-D</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2695,8 +2695,8 @@
         <v>212</v>
       </c>
       <c r="D97" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>26D</v>
+        <f t="shared" si="1"/>
+        <v>26-D</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2707,7 +2707,7 @@
         <v>173</v>
       </c>
       <c r="D98" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
     </row>
@@ -2719,7 +2719,7 @@
         <v>173</v>
       </c>
       <c r="D99" s="3" t="str">
-        <f t="shared" ref="D99" si="3">_xlfn.CONCAT(B99,C99)</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
     </row>
@@ -2731,7 +2731,7 @@
         <v>173</v>
       </c>
       <c r="D100" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
     </row>
@@ -2743,7 +2743,7 @@
         <v>173</v>
       </c>
       <c r="D101" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
     </row>
@@ -2755,7 +2755,7 @@
         <v>173</v>
       </c>
       <c r="D102" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
     </row>
@@ -2767,7 +2767,7 @@
         <v>173</v>
       </c>
       <c r="D103" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
     </row>
@@ -2779,7 +2779,7 @@
         <v>289</v>
       </c>
       <c r="D104" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
     </row>
@@ -2791,7 +2791,7 @@
         <v>171</v>
       </c>
       <c r="D105" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
     </row>
@@ -2803,7 +2803,7 @@
         <v>171</v>
       </c>
       <c r="D106" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
     </row>
@@ -2815,7 +2815,7 @@
         <v>207</v>
       </c>
       <c r="D107" s="3" t="str">
-        <f t="shared" ref="D107" si="4">_xlfn.CONCAT(B107,C107)</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -2827,7 +2827,7 @@
         <v>207</v>
       </c>
       <c r="D108" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -2839,7 +2839,7 @@
         <v>207</v>
       </c>
       <c r="D109" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -2851,7 +2851,7 @@
         <v>207</v>
       </c>
       <c r="D110" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -2863,7 +2863,7 @@
         <v>207</v>
       </c>
       <c r="D111" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -2875,7 +2875,7 @@
         <v>207</v>
       </c>
       <c r="D112" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -2887,7 +2887,7 @@
         <v>265</v>
       </c>
       <c r="D113" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
     </row>
@@ -2899,7 +2899,7 @@
         <v>242</v>
       </c>
       <c r="D114" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
     </row>
@@ -2914,8 +2914,8 @@
         <v>256</v>
       </c>
       <c r="D115" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>16SC</v>
+        <f>IF(C115 &lt;&gt; "",_xlfn.CONCAT(B115,_xlfn.CONCAT("-",C115)),B115)</f>
+        <v>16-SC</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2926,7 +2926,7 @@
         <v>204</v>
       </c>
       <c r="D116" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D116:D179" si="2">IF(C116 &lt;&gt; "",_xlfn.CONCAT(B116,_xlfn.CONCAT("-",C116)),B116)</f>
         <v>32</v>
       </c>
     </row>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="D122" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>35BS</v>
+        <v>35-BS</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -3017,7 +3017,7 @@
       </c>
       <c r="D123" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>35CC</v>
+        <v>35-CC</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -3031,8 +3031,8 @@
         <v>182</v>
       </c>
       <c r="D124" s="3" t="str">
-        <f t="shared" ref="D124:D163" si="5">_xlfn.CONCAT(B124,C124)</f>
-        <v>35CC</v>
+        <f t="shared" si="2"/>
+        <v>35-CC</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3046,8 +3046,8 @@
         <v>192</v>
       </c>
       <c r="D125" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35EB</v>
+        <f t="shared" si="2"/>
+        <v>35-EB</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -3061,8 +3061,8 @@
         <v>192</v>
       </c>
       <c r="D126" s="3" t="str">
-        <f t="shared" ref="D126" si="6">_xlfn.CONCAT(B126,C126)</f>
-        <v>35EB</v>
+        <f t="shared" si="2"/>
+        <v>35-EB</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -3076,8 +3076,8 @@
         <v>192</v>
       </c>
       <c r="D127" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35EB</v>
+        <f t="shared" si="2"/>
+        <v>35-EB</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -3091,8 +3091,8 @@
         <v>192</v>
       </c>
       <c r="D128" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35EB</v>
+        <f t="shared" si="2"/>
+        <v>35-EB</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -3106,8 +3106,8 @@
         <v>192</v>
       </c>
       <c r="D129" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35EB</v>
+        <f t="shared" si="2"/>
+        <v>35-EB</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -3121,8 +3121,8 @@
         <v>193</v>
       </c>
       <c r="D130" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35HA</v>
+        <f t="shared" si="2"/>
+        <v>35-HA</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -3136,8 +3136,8 @@
         <v>193</v>
       </c>
       <c r="D131" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35HA</v>
+        <f t="shared" si="2"/>
+        <v>35-HA</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -3151,8 +3151,8 @@
         <v>194</v>
       </c>
       <c r="D132" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35IN</v>
+        <f t="shared" si="2"/>
+        <v>35-IN</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -3166,8 +3166,8 @@
         <v>194</v>
       </c>
       <c r="D133" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35IN</v>
+        <f t="shared" si="2"/>
+        <v>35-IN</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -3181,8 +3181,8 @@
         <v>194</v>
       </c>
       <c r="D134" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35IN</v>
+        <f t="shared" si="2"/>
+        <v>35-IN</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3196,8 +3196,8 @@
         <v>195</v>
       </c>
       <c r="D135" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35PGW</v>
+        <f t="shared" si="2"/>
+        <v>35-PGW</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -3211,8 +3211,8 @@
         <v>195</v>
       </c>
       <c r="D136" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35PGW</v>
+        <f t="shared" si="2"/>
+        <v>35-PGW</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -3226,8 +3226,8 @@
         <v>195</v>
       </c>
       <c r="D137" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35PGW</v>
+        <f t="shared" si="2"/>
+        <v>35-PGW</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -3241,8 +3241,8 @@
         <v>196</v>
       </c>
       <c r="D138" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35R</v>
+        <f t="shared" si="2"/>
+        <v>35-R</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -3256,8 +3256,8 @@
         <v>196</v>
       </c>
       <c r="D139" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35R</v>
+        <f t="shared" si="2"/>
+        <v>35-R</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -3271,8 +3271,8 @@
         <v>197</v>
       </c>
       <c r="D140" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35R32</v>
+        <f t="shared" si="2"/>
+        <v>35-R32</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -3286,8 +3286,8 @@
         <v>197</v>
       </c>
       <c r="D141" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35R32</v>
+        <f t="shared" si="2"/>
+        <v>35-R32</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -3301,8 +3301,8 @@
         <v>191</v>
       </c>
       <c r="D142" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35SD</v>
+        <f t="shared" si="2"/>
+        <v>35-SD</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -3316,8 +3316,8 @@
         <v>191</v>
       </c>
       <c r="D143" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35SD</v>
+        <f t="shared" si="2"/>
+        <v>35-SD</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -3331,8 +3331,8 @@
         <v>191</v>
       </c>
       <c r="D144" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35SD</v>
+        <f t="shared" si="2"/>
+        <v>35-SD</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -3346,8 +3346,8 @@
         <v>191</v>
       </c>
       <c r="D145" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35SD</v>
+        <f t="shared" si="2"/>
+        <v>35-SD</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -3361,8 +3361,8 @@
         <v>191</v>
       </c>
       <c r="D146" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35SD</v>
+        <f t="shared" si="2"/>
+        <v>35-SD</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -3376,8 +3376,8 @@
         <v>198</v>
       </c>
       <c r="D147" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35WF</v>
+        <f t="shared" si="2"/>
+        <v>35-WF</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3391,8 +3391,8 @@
         <v>198</v>
       </c>
       <c r="D148" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35WF</v>
+        <f t="shared" si="2"/>
+        <v>35-WF</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3406,8 +3406,8 @@
         <v>269</v>
       </c>
       <c r="D149" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35BSR</v>
+        <f t="shared" si="2"/>
+        <v>35-BSR</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3421,8 +3421,8 @@
         <v>272</v>
       </c>
       <c r="D150" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35RR</v>
+        <f t="shared" si="2"/>
+        <v>35-RR</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3436,8 +3436,8 @@
         <v>283</v>
       </c>
       <c r="D151" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>35FGR</v>
+        <f t="shared" si="2"/>
+        <v>35-FGR</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -3448,7 +3448,7 @@
         <v>244</v>
       </c>
       <c r="D152" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
     </row>
@@ -3460,7 +3460,7 @@
         <v>185</v>
       </c>
       <c r="D153" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
     </row>
@@ -3472,7 +3472,7 @@
         <v>185</v>
       </c>
       <c r="D154" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
     </row>
@@ -3484,7 +3484,7 @@
         <v>185</v>
       </c>
       <c r="D155" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
     </row>
@@ -3496,7 +3496,7 @@
         <v>185</v>
       </c>
       <c r="D156" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
     </row>
@@ -3508,7 +3508,7 @@
         <v>235</v>
       </c>
       <c r="D157" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
     </row>
@@ -3520,7 +3520,7 @@
         <v>179</v>
       </c>
       <c r="D158" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
     </row>
@@ -3532,7 +3532,7 @@
         <v>178</v>
       </c>
       <c r="D159" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
     </row>
@@ -3544,7 +3544,7 @@
         <v>178</v>
       </c>
       <c r="D160" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
     </row>
@@ -3556,7 +3556,7 @@
         <v>178</v>
       </c>
       <c r="D161" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
     </row>
@@ -3568,7 +3568,7 @@
         <v>178</v>
       </c>
       <c r="D162" s="3" t="str">
-        <f t="shared" ref="D162" si="7">_xlfn.CONCAT(B162,C162)</f>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
     </row>
@@ -3580,7 +3580,7 @@
         <v>181</v>
       </c>
       <c r="D163" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
     </row>
@@ -3595,8 +3595,8 @@
         <v>182</v>
       </c>
       <c r="D164" s="3" t="str">
-        <f t="shared" ref="D164:D202" si="8">_xlfn.CONCAT(B164,C164)</f>
-        <v>42CC</v>
+        <f t="shared" si="2"/>
+        <v>42-CC</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -3610,8 +3610,8 @@
         <v>182</v>
       </c>
       <c r="D165" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v>42CC</v>
+        <f t="shared" si="2"/>
+        <v>42-CC</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -3625,8 +3625,8 @@
         <v>183</v>
       </c>
       <c r="D166" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v>42ES</v>
+        <f t="shared" si="2"/>
+        <v>42-ES</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -3637,7 +3637,7 @@
         <v>264</v>
       </c>
       <c r="D167" s="3" t="str">
-        <f>_xlfn.CONCAT(B167,C167)</f>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
     </row>
@@ -3649,7 +3649,7 @@
         <v>209</v>
       </c>
       <c r="D168" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
     </row>
@@ -3661,7 +3661,7 @@
         <v>172</v>
       </c>
       <c r="D169" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
     </row>
@@ -3673,7 +3673,7 @@
         <v>220</v>
       </c>
       <c r="D170" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
     </row>
@@ -3685,7 +3685,7 @@
         <v>220</v>
       </c>
       <c r="D171" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
     </row>
@@ -3697,7 +3697,7 @@
         <v>220</v>
       </c>
       <c r="D172" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
     </row>
@@ -3709,7 +3709,7 @@
         <v>220</v>
       </c>
       <c r="D173" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
     </row>
@@ -3721,7 +3721,7 @@
         <v>247</v>
       </c>
       <c r="D174" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
     </row>
@@ -3733,7 +3733,7 @@
         <v>229</v>
       </c>
       <c r="D175" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
     </row>
@@ -3745,7 +3745,7 @@
         <v>229</v>
       </c>
       <c r="D176" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
     </row>
@@ -3757,7 +3757,7 @@
         <v>229</v>
       </c>
       <c r="D177" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
     </row>
@@ -3769,7 +3769,7 @@
         <v>228</v>
       </c>
       <c r="D178" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
     </row>
@@ -3781,7 +3781,7 @@
         <v>213</v>
       </c>
       <c r="D179" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
     </row>
@@ -3793,7 +3793,7 @@
         <v>213</v>
       </c>
       <c r="D180" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="D180:D225" si="3">IF(C180 &lt;&gt; "",_xlfn.CONCAT(B180,_xlfn.CONCAT("-",C180)),B180)</f>
         <v>50</v>
       </c>
     </row>
@@ -3805,7 +3805,7 @@
         <v>213</v>
       </c>
       <c r="D181" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
     </row>
@@ -3817,7 +3817,7 @@
         <v>177</v>
       </c>
       <c r="D182" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
     </row>
@@ -3829,7 +3829,7 @@
         <v>177</v>
       </c>
       <c r="D183" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
     </row>
@@ -3841,7 +3841,7 @@
         <v>203</v>
       </c>
       <c r="D184" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>52</v>
       </c>
     </row>
@@ -3853,7 +3853,7 @@
         <v>316</v>
       </c>
       <c r="D185" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>53</v>
       </c>
     </row>
@@ -3865,7 +3865,7 @@
         <v>205</v>
       </c>
       <c r="D186" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
     </row>
@@ -3877,7 +3877,7 @@
         <v>205</v>
       </c>
       <c r="D187" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
     </row>
@@ -3889,7 +3889,7 @@
         <v>180</v>
       </c>
       <c r="D188" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
     </row>
@@ -3901,7 +3901,7 @@
         <v>180</v>
       </c>
       <c r="D189" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
     </row>
@@ -3913,7 +3913,7 @@
         <v>180</v>
       </c>
       <c r="D190" s="3" t="str">
-        <f t="shared" ref="D190" si="9">_xlfn.CONCAT(B190,C190)</f>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
     </row>
@@ -3925,7 +3925,7 @@
         <v>225</v>
       </c>
       <c r="D191" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
     </row>
@@ -3937,7 +3937,7 @@
         <v>225</v>
       </c>
       <c r="D192" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
     </row>
@@ -3949,7 +3949,7 @@
         <v>248</v>
       </c>
       <c r="D193" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
     </row>
@@ -3961,7 +3961,7 @@
         <v>248</v>
       </c>
       <c r="D194" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
     </row>
@@ -3973,7 +3973,7 @@
         <v>248</v>
       </c>
       <c r="D195" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
     </row>
@@ -3985,7 +3985,7 @@
         <v>248</v>
       </c>
       <c r="D196" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
     </row>
@@ -3997,7 +3997,7 @@
         <v>248</v>
       </c>
       <c r="D197" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
     </row>
@@ -4009,7 +4009,7 @@
         <v>248</v>
       </c>
       <c r="D198" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
     </row>
@@ -4021,7 +4021,7 @@
         <v>248</v>
       </c>
       <c r="D199" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
     </row>
@@ -4033,7 +4033,7 @@
         <v>248</v>
       </c>
       <c r="D200" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
     </row>
@@ -4045,7 +4045,7 @@
         <v>248</v>
       </c>
       <c r="D201" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
     </row>
@@ -4057,7 +4057,7 @@
         <v>227</v>
       </c>
       <c r="D202" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>59</v>
       </c>
     </row>
@@ -4069,7 +4069,7 @@
         <v>170</v>
       </c>
       <c r="D203" s="3" t="str">
-        <f t="shared" ref="D203:D228" si="10">_xlfn.CONCAT(B203,C203)</f>
+        <f t="shared" si="3"/>
         <v>61</v>
       </c>
     </row>
@@ -4081,7 +4081,7 @@
         <v>170</v>
       </c>
       <c r="D204" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>61</v>
       </c>
     </row>
@@ -4093,7 +4093,7 @@
         <v>170</v>
       </c>
       <c r="D205" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>61</v>
       </c>
     </row>
@@ -4105,7 +4105,7 @@
         <v>216</v>
       </c>
       <c r="D206" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>62</v>
       </c>
     </row>
@@ -4117,7 +4117,7 @@
         <v>216</v>
       </c>
       <c r="D207" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>62</v>
       </c>
     </row>
@@ -4129,7 +4129,7 @@
         <v>174</v>
       </c>
       <c r="D208" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
     </row>
@@ -4141,7 +4141,7 @@
         <v>174</v>
       </c>
       <c r="D209" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
     </row>
@@ -4153,7 +4153,7 @@
         <v>174</v>
       </c>
       <c r="D210" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
     </row>
@@ -4165,7 +4165,7 @@
         <v>215</v>
       </c>
       <c r="D211" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
     </row>
@@ -4177,7 +4177,7 @@
         <v>215</v>
       </c>
       <c r="D212" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
     </row>
@@ -4189,7 +4189,7 @@
         <v>214</v>
       </c>
       <c r="D213" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
     </row>
@@ -4201,7 +4201,7 @@
         <v>214</v>
       </c>
       <c r="D214" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
     </row>
@@ -4213,7 +4213,7 @@
         <v>214</v>
       </c>
       <c r="D215" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
     </row>
@@ -4225,7 +4225,7 @@
         <v>214</v>
       </c>
       <c r="D216" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
     </row>
@@ -4237,7 +4237,7 @@
         <v>214</v>
       </c>
       <c r="D217" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
     </row>
@@ -4249,7 +4249,7 @@
         <v>291</v>
       </c>
       <c r="D218" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>67</v>
       </c>
     </row>
@@ -4261,7 +4261,7 @@
         <v>243</v>
       </c>
       <c r="D219" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>68</v>
       </c>
     </row>
@@ -4273,7 +4273,7 @@
         <v>187</v>
       </c>
       <c r="D220" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>69</v>
       </c>
     </row>
@@ -4285,7 +4285,7 @@
         <v>245</v>
       </c>
       <c r="D221" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
     </row>
@@ -4297,7 +4297,7 @@
         <v>232</v>
       </c>
       <c r="D222" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
     </row>
@@ -4309,7 +4309,7 @@
         <v>175</v>
       </c>
       <c r="D223" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>73</v>
       </c>
     </row>
@@ -4321,7 +4321,7 @@
         <v>175</v>
       </c>
       <c r="D224" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>73</v>
       </c>
     </row>
@@ -4333,7 +4333,7 @@
         <v>200</v>
       </c>
       <c r="D225" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>84</v>
       </c>
     </row>
@@ -4341,7 +4341,7 @@
       <c r="B226"/>
       <c r="C226"/>
       <c r="D226" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="D203:D228" si="4">_xlfn.CONCAT(B226,C226)</f>
         <v/>
       </c>
     </row>
@@ -4349,7 +4349,7 @@
       <c r="B227"/>
       <c r="C227"/>
       <c r="D227" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -4357,7 +4357,7 @@
       <c r="B228"/>
       <c r="C228"/>
       <c r="D228" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
fix bug in CAO
</commit_message>
<xml_diff>
--- a/billy_penn/data/dept_names_lookup.xlsx
+++ b/billy_penn/data/dept_names_lookup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/Software/billy-penn/billy_penn/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C09160-6D52-1F43-A2A4-478785D0A2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F694728A-641C-4F41-B883-E1647439DF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1429,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D228"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A195" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D210" sqref="D210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4150,11 +4150,11 @@
         <v>298</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>174</v>
+        <v>215</v>
       </c>
       <c r="D210" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -4341,7 +4341,7 @@
       <c r="B226"/>
       <c r="C226"/>
       <c r="D226" s="3" t="str">
-        <f t="shared" ref="D203:D228" si="4">_xlfn.CONCAT(B226,C226)</f>
+        <f t="shared" ref="D226:D228" si="4">_xlfn.CONCAT(B226,C226)</f>
         <v/>
       </c>
     </row>

</xml_diff>